<commit_message>
Alteracao - Telas nob=vas 1
</commit_message>
<xml_diff>
--- a/Verithus/Documentação/Relação de Procedures.xlsx
+++ b/Verithus/Documentação/Relação de Procedures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="82">
   <si>
     <t>SEQ</t>
   </si>
@@ -248,37 +248,28 @@
     <t>SPVRT066_FERIAS_PR_ALTERAR</t>
   </si>
   <si>
-    <t>SPVRT067_FERIAS_PR_EXCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT068_FERIAS_PR_INCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT069_FERIAS_PR_SELECIONAR</t>
-  </si>
-  <si>
-    <t>SPVRT070_ACIDENTE_TRABALHO_PR_ALTERAR</t>
-  </si>
-  <si>
-    <t>SPVRT071_ACIDENTE_TRABALHO_PR_EXCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT072_ACIDENTE_TRABALHO_PR_INCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT073_ACIDENTE_TRABALHO_PR_SELECIONAR</t>
-  </si>
-  <si>
-    <t>SPVRT074_ALTERACAO_CARGO_SALARIO_PR_ALTERAR</t>
-  </si>
-  <si>
-    <t>SPVRT075_ALTERACAO_CARGO_SALARIO_PR_EXCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT076_ALTERACAO_CARGO_SALARIO_PR_INCLUIR</t>
-  </si>
-  <si>
-    <t>SPVRT077_ALTERACAO_CARGO_SALARIO_PR_SELECIONAR</t>
+    <t>SPVRT067_FERIAS_PR_INCLUIR</t>
+  </si>
+  <si>
+    <t>SPVRT068_FERIAS_PR_SELECIONAR</t>
+  </si>
+  <si>
+    <t>SPVRT069_ACIDENTE_TRABALHO_PR_ALTERAR</t>
+  </si>
+  <si>
+    <t>SPVRT070_ACIDENTE_TRABALHO_PR_INCLUIR</t>
+  </si>
+  <si>
+    <t>SPVRT071_ACIDENTE_TRABALHO_PR_SELECIONAR</t>
+  </si>
+  <si>
+    <t>SPVRT072_ALTERACAO_CARGO_SALARIO_PR_ALTERAR</t>
+  </si>
+  <si>
+    <t>SPVRT073_ALTERACAO_CARGO_SALARIO_PR_INCLUIR</t>
+  </si>
+  <si>
+    <t>SPVRT074_ALTERACAO_CARGO_SALARIO_PR_SELECIONAR</t>
   </si>
 </sst>
 </file>
@@ -431,8 +422,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="A1:C78" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="A1:C75" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C75"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SEQ" dataDxfId="2"/>
     <tableColumn id="2" name="NOME PROC" dataDxfId="1"/>
@@ -705,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,7 +1454,7 @@
         <v>74</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1474,18 +1465,18 @@
         <v>75</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1496,7 +1487,7 @@
         <v>77</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +1498,7 @@
         <v>78</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,7 +1509,7 @@
         <v>79</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1529,7 +1520,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,39 +1531,6 @@
         <v>81</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>76</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>77</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>